<commit_message>
save before deleting bball ref implementation
</commit_message>
<xml_diff>
--- a/MLB_2017-08-08.xlsx
+++ b/MLB_2017-08-08.xlsx
@@ -259,52 +259,52 @@
     <t>FORM</t>
   </si>
   <si>
+    <t>AWAY:  Miami Marlins</t>
+  </si>
+  <si>
     <t>HOME:  Washington Nationals</t>
   </si>
   <si>
-    <t>AWAY:  Miami Marlins</t>
+    <t>AWAY:  Detroit Tigers</t>
   </si>
   <si>
     <t>HOME:  Pittsburgh Pirates</t>
   </si>
   <si>
-    <t>AWAY:  Detroit Tigers</t>
+    <t>AWAY:  New York Yankees</t>
   </si>
   <si>
     <t>HOME:  Toronto Blue Jays</t>
   </si>
   <si>
-    <t>AWAY:  New York Yankees</t>
+    <t>AWAY:  Colorado Rockies</t>
   </si>
   <si>
     <t>HOME:  Cleveland Indians</t>
   </si>
   <si>
-    <t>AWAY:  Colorado Rockies</t>
+    <t>AWAY:  San Diego Padres</t>
   </si>
   <si>
     <t>HOME:  Cincinnati Reds</t>
   </si>
   <si>
-    <t>AWAY:  San Diego Padres</t>
+    <t>AWAY:  Texas Rangers</t>
   </si>
   <si>
     <t>HOME:  New York Mets</t>
   </si>
   <si>
-    <t>AWAY:  Texas Rangers</t>
+    <t>AWAY:  Boston Red Sox</t>
   </si>
   <si>
     <t>HOME:  Tampa Bay Rays</t>
   </si>
   <si>
-    <t>AWAY:  Boston Red Sox</t>
+    <t>AWAY:  Philadelphia Phillies</t>
   </si>
   <si>
     <t>HOME:  Atlanta Braves</t>
-  </si>
-  <si>
-    <t>AWAY:  Philadelphia Phillies</t>
   </si>
   <si>
     <t>RESULT</t>
@@ -316,6 +316,12 @@
     <t>6</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>14</t>
   </si>
   <si>
@@ -325,16 +331,10 @@
     <t>5</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>11</t>
   </si>
   <si>
     <t>4</t>
-  </si>
-  <si>
-    <t>11</t>
   </si>
   <si>
     <t>9</t>
@@ -607,54 +607,6 @@
     <t>H V A</t>
   </si>
   <si>
-    <t>4.91</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>9.00</t>
-  </si>
-  <si>
-    <t>4.53</t>
-  </si>
-  <si>
-    <t>3.92</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>1.50</t>
-  </si>
-  <si>
-    <t>2.77</t>
-  </si>
-  <si>
-    <t>4.88</t>
-  </si>
-  <si>
-    <t>12.00</t>
-  </si>
-  <si>
-    <t>5.65</t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>13.50</t>
-  </si>
-  <si>
-    <t>5.10</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>15.43</t>
-  </si>
-  <si>
     <t>5.31</t>
   </si>
   <si>
@@ -709,6 +661,54 @@
     <t>1.29</t>
   </si>
   <si>
+    <t>4.91</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>9.00</t>
+  </si>
+  <si>
+    <t>4.53</t>
+  </si>
+  <si>
+    <t>3.92</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>2.77</t>
+  </si>
+  <si>
+    <t>4.88</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>5.65</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>13.50</t>
+  </si>
+  <si>
+    <t>5.10</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>15.43</t>
+  </si>
+  <si>
     <t>QUAL-RATE</t>
   </si>
   <si>
@@ -739,46 +739,46 @@
     <t>ADDITTIONS</t>
   </si>
   <si>
+    <t>AWAY:  Houston Astros</t>
+  </si>
+  <si>
     <t>HOME:  Chicago White Sox</t>
   </si>
   <si>
-    <t>AWAY:  Houston Astros</t>
+    <t>AWAY:  Milwaukee Brewers</t>
   </si>
   <si>
     <t>HOME:  Minnesota Twins</t>
   </si>
   <si>
-    <t>AWAY:  Milwaukee Brewers</t>
+    <t>AWAY:  St. Louis Cardinals</t>
   </si>
   <si>
     <t>HOME:  Kansas City Royals</t>
   </si>
   <si>
-    <t>AWAY:  St. Louis Cardinals</t>
+    <t>AWAY:  Los Angeles Dodgers</t>
   </si>
   <si>
     <t>HOME:  Arizona Diamondbacks</t>
   </si>
   <si>
-    <t>AWAY:  Los Angeles Dodgers</t>
+    <t>AWAY:  Seattle Mariners</t>
   </si>
   <si>
     <t>HOME:  Oakland Athletics</t>
   </si>
   <si>
-    <t>AWAY:  Seattle Mariners</t>
+    <t>AWAY:  Baltimore Orioles</t>
   </si>
   <si>
     <t>HOME:  Los Angeles Angels</t>
   </si>
   <si>
-    <t>AWAY:  Baltimore Orioles</t>
+    <t>AWAY:  Chicago Cubs</t>
   </si>
   <si>
     <t>HOME:  San Francisco Giants</t>
-  </si>
-  <si>
-    <t>AWAY:  Chicago Cubs</t>
   </si>
   <si>
     <t>3712</t>
@@ -922,6 +922,33 @@
     <t>38</t>
   </si>
   <si>
+    <t>2.15</t>
+  </si>
+  <si>
+    <t>3.68</t>
+  </si>
+  <si>
+    <t>3.66</t>
+  </si>
+  <si>
+    <t>3.79</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>4.41</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>4.45</t>
+  </si>
+  <si>
+    <t>4.42</t>
+  </si>
+  <si>
     <t>5.27</t>
   </si>
   <si>
@@ -950,33 +977,6 @@
   </si>
   <si>
     <t>3.86</t>
-  </si>
-  <si>
-    <t>2.15</t>
-  </si>
-  <si>
-    <t>3.68</t>
-  </si>
-  <si>
-    <t>3.66</t>
-  </si>
-  <si>
-    <t>3.79</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
-    <t>4.41</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>4.45</t>
-  </si>
-  <si>
-    <t>4.42</t>
   </si>
   <si>
     <t>QUAL PROF</t>
@@ -1767,8 +1767,8 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="191">
@@ -2229,8 +2229,8 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="1"/>
     <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="2"/>
   </cellStyles>
   <dxfs count="2022">
@@ -32744,13 +32744,13 @@
         <v>9</v>
       </c>
       <c r="M10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O10" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P10" s="165" t="n"/>
       <c r="Q10" s="7" t="s">
@@ -32760,13 +32760,13 @@
         <v>9</v>
       </c>
       <c r="S10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U10" s="38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V10" s="14" t="n"/>
       <c r="W10" s="165" t="n"/>
@@ -32781,10 +32781,10 @@
         <v>9</v>
       </c>
       <c r="AB10" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC10" s="38" t="s">
         <v>8</v>
-      </c>
-      <c r="AC10" s="38" t="s">
-        <v>9</v>
       </c>
       <c r="AD10" s="165" t="n"/>
       <c r="AE10" s="7" t="s">
@@ -32797,10 +32797,10 @@
         <v>9</v>
       </c>
       <c r="AH10" s="154" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI10" s="38" t="s">
         <v>9</v>
-      </c>
-      <c r="AI10" s="38" t="s">
-        <v>8</v>
       </c>
       <c r="AJ10" s="14" t="n"/>
       <c r="AL10" s="13" t="n"/>
@@ -32808,32 +32808,32 @@
         <v>96</v>
       </c>
       <c r="AN10" s="154" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO10" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="AO10" s="154" t="s">
+      <c r="AP10" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ10" s="38" t="s">
         <v>8</v>
-      </c>
-      <c r="AP10" s="154" t="s">
-        <v>8</v>
-      </c>
-      <c r="AQ10" s="38" t="s">
-        <v>9</v>
       </c>
       <c r="AR10" s="165" t="n"/>
       <c r="AS10" s="7" t="s">
         <v>96</v>
       </c>
       <c r="AT10" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU10" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="AU10" s="154" t="s">
+      <c r="AV10" s="154" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW10" s="38" t="s">
         <v>9</v>
-      </c>
-      <c r="AV10" s="154" t="s">
-        <v>9</v>
-      </c>
-      <c r="AW10" s="38" t="s">
-        <v>8</v>
       </c>
       <c r="AX10" s="14" t="n"/>
       <c r="AZ10" s="13" t="n"/>
@@ -32844,7 +32844,7 @@
         <v>9</v>
       </c>
       <c r="BC10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD10" s="154" t="s">
         <v>8</v>
@@ -32860,7 +32860,7 @@
         <v>9</v>
       </c>
       <c r="BI10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BJ10" s="154" t="s">
         <v>8</v>
@@ -32877,10 +32877,10 @@
         <v>8</v>
       </c>
       <c r="BQ10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BR10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BS10" s="38" t="s">
         <v>8</v>
@@ -32893,10 +32893,10 @@
         <v>8</v>
       </c>
       <c r="BW10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BX10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BY10" s="38" t="s">
         <v>8</v>
@@ -32947,7 +32947,7 @@
         <v>8</v>
       </c>
       <c r="CT10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="CU10" s="38" t="s">
         <v>9</v>
@@ -32963,7 +32963,7 @@
         <v>8</v>
       </c>
       <c r="CZ10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="DA10" s="38" t="s">
         <v>9</v>
@@ -32980,10 +32980,10 @@
         <v>9</v>
       </c>
       <c r="DH10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="DI10" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="DJ10" s="165" t="n"/>
       <c r="DK10" s="7" t="s">
@@ -32996,10 +32996,10 @@
         <v>9</v>
       </c>
       <c r="DN10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="DO10" s="38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="DP10" s="14" t="n"/>
       <c r="DR10" s="47" t="n"/>
@@ -33037,7 +33037,7 @@
         <v>100</v>
       </c>
       <c r="O11" s="144" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P11" s="75" t="n"/>
       <c r="Q11" s="143" t="s">
@@ -33047,13 +33047,13 @@
         <v>98</v>
       </c>
       <c r="S11" s="156" t="s">
+        <v>101</v>
+      </c>
+      <c r="T11" s="156" t="s">
         <v>102</v>
       </c>
-      <c r="T11" s="156" t="s">
+      <c r="U11" s="144" t="s">
         <v>103</v>
-      </c>
-      <c r="U11" s="144" t="s">
-        <v>98</v>
       </c>
       <c r="V11" s="14" t="n"/>
       <c r="W11" s="75" t="n"/>
@@ -33062,26 +33062,26 @@
         <v>97</v>
       </c>
       <c r="Z11" s="156" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AA11" s="156" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AB11" s="156" t="s">
         <v>104</v>
       </c>
       <c r="AC11" s="144" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD11" s="75" t="n"/>
       <c r="AE11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="AF11" s="156" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="AG11" s="156" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="AH11" s="156" t="s">
         <v>105</v>
@@ -33095,10 +33095,10 @@
         <v>97</v>
       </c>
       <c r="AN11" s="156" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AO11" s="156" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AP11" s="156" t="s">
         <v>105</v>
@@ -33111,16 +33111,16 @@
         <v>97</v>
       </c>
       <c r="AT11" s="156" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AU11" s="156" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="AV11" s="156" t="s">
         <v>104</v>
       </c>
       <c r="AW11" s="144" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX11" s="14" t="n"/>
       <c r="AZ11" s="13" t="n"/>
@@ -33128,13 +33128,13 @@
         <v>97</v>
       </c>
       <c r="BB11" s="156" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="BC11" s="156" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="BD11" s="156" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="BE11" s="144" t="s">
         <v>101</v>
@@ -33144,16 +33144,16 @@
         <v>97</v>
       </c>
       <c r="BH11" s="156" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="BI11" s="156" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="BJ11" s="156" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="BK11" s="144" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="BL11" s="14" t="n"/>
       <c r="BN11" s="13" t="n"/>
@@ -33161,32 +33161,32 @@
         <v>97</v>
       </c>
       <c r="BP11" s="156" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="BQ11" s="156" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BR11" s="156" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="BS11" s="144" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="BT11" s="75" t="n"/>
       <c r="BU11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="BV11" s="156" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="BW11" s="156" t="s">
+        <v>101</v>
+      </c>
+      <c r="BX11" s="156" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY11" s="144" t="s">
         <v>103</v>
-      </c>
-      <c r="BX11" s="156" t="s">
-        <v>101</v>
-      </c>
-      <c r="BY11" s="144" t="s">
-        <v>101</v>
       </c>
       <c r="BZ11" s="14" t="n"/>
       <c r="CA11" s="75" t="n"/>
@@ -33195,29 +33195,29 @@
         <v>97</v>
       </c>
       <c r="CD11" s="156" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="CE11" s="156" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="CF11" s="156" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="CG11" s="144" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="CH11" s="75" t="n"/>
       <c r="CI11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="CJ11" s="156" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="CK11" s="156" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="CL11" s="156" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="CM11" s="144" t="s">
         <v>101</v>
@@ -33228,32 +33228,32 @@
         <v>97</v>
       </c>
       <c r="CR11" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CS11" s="156" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="CT11" s="156" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="CU11" s="144" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="CV11" s="75" t="n"/>
       <c r="CW11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="CX11" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CY11" s="156" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="CZ11" s="156" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="DA11" s="144" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="DB11" s="14" t="n"/>
       <c r="DD11" s="13" t="n"/>
@@ -33261,32 +33261,32 @@
         <v>97</v>
       </c>
       <c r="DF11" s="156" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="DG11" s="156" t="s">
         <v>103</v>
       </c>
       <c r="DH11" s="156" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="DI11" s="144" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="DJ11" s="75" t="n"/>
       <c r="DK11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="DL11" s="156" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="DM11" s="156" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="DN11" s="156" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="DO11" s="144" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="DP11" s="14" t="n"/>
       <c r="EE11" s="75" t="n"/>
@@ -36938,7 +36938,7 @@
         <v>109</v>
       </c>
       <c r="AA31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AB31" s="172">
         <f>IF((Z31+AA31)&lt;4,IF(AD4="POS",0.7,IF(AD4="NEUT",0.5,IF(AD4="NEG",0.3,""))),Z31/(Z31+AA31))</f>
@@ -36951,7 +36951,7 @@
         <v>109</v>
       </c>
       <c r="AH31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AI31" s="172">
         <f>IF((AG31+AH31)&lt;4,IF(AD5="POS",0.7,IF(AD5="NEUT",0.5,IF(AD5="NEG",0.3,""))),AG31/(AG31+AH31))</f>
@@ -36966,7 +36966,7 @@
         <v>108</v>
       </c>
       <c r="AO31" s="154" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AP31" s="172">
         <f>IF((AN31+AO31)&lt;4,IF(AR4="POS",0.7,IF(AR4="NEUT",0.5,IF(AR4="NEG",0.3,""))),AN31/(AN31+AO31))</f>
@@ -36979,7 +36979,7 @@
         <v>108</v>
       </c>
       <c r="AV31" s="154" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AW31" s="172">
         <f>IF((AU31+AV31)&lt;4,IF(AR5="POS",0.7,IF(AR5="NEUT",0.5,IF(AR5="NEG",0.3,""))),AU31/(AU31+AV31))</f>
@@ -36991,7 +36991,7 @@
         <v>137</v>
       </c>
       <c r="BB31" s="154" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="BC31" s="154" t="s">
         <v>108</v>
@@ -37004,7 +37004,7 @@
         <v>137</v>
       </c>
       <c r="BI31" s="154" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="BJ31" s="154" t="s">
         <v>108</v>
@@ -37075,7 +37075,7 @@
         <v>137</v>
       </c>
       <c r="CR31" s="154" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CS31" s="154" t="s">
         <v>108</v>
@@ -37088,7 +37088,7 @@
         <v>137</v>
       </c>
       <c r="CY31" s="154" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CZ31" s="154" t="s">
         <v>108</v>
@@ -37106,7 +37106,7 @@
         <v>108</v>
       </c>
       <c r="DG31" s="154" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="DH31" s="172">
         <f>IF((DF31+DG31)&lt;4,IF(DJ4="POS",0.7,IF(DJ4="NEUT",0.5,IF(DJ4="NEG",0.3,""))),DF31/(DF31+DG31))</f>
@@ -37119,7 +37119,7 @@
         <v>108</v>
       </c>
       <c r="DN31" s="154" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="DO31" s="172">
         <f>IF((DM31+DN31)&lt;4,IF(DJ5="POS",0.7,IF(DJ5="NEUT",0.5,IF(DJ5="NEG",0.3,""))),DM31/(DM31+DN31))</f>
@@ -37189,7 +37189,7 @@
         <v>109</v>
       </c>
       <c r="AA32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AB32" s="170">
         <f>IF((Z32+AA32)&lt;4,IF(AD4="POS",0.7,IF(AD4="NEUT",0.5,IF(AD4="NEG",0.3,""))),Z32/(Z32+AA32))</f>
@@ -37202,7 +37202,7 @@
         <v>109</v>
       </c>
       <c r="AH32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AI32" s="170">
         <f>IF((AG32+AH32)&lt;4,IF(AD5="POS",0.7,IF(AD5="NEUT",0.5,IF(AD5="NEG",0.3,""))),AG32/(AG32+AH32))</f>
@@ -37214,10 +37214,10 @@
         <v>154</v>
       </c>
       <c r="AN32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AO32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AP32" s="170">
         <f>IF((AN32+AO32)&lt;4,IF(AR4="POS",0.7,IF(AR4="NEUT",0.5,IF(AR4="NEG",0.3,""))),AN32/(AN32+AO32))</f>
@@ -37227,10 +37227,10 @@
         <v>154</v>
       </c>
       <c r="AU32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AV32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AW32" s="170">
         <f>IF((AU32+AV32)&lt;4,IF(AR5="POS",0.7,IF(AR5="NEUT",0.5,IF(AR5="NEG",0.3,""))),AU32/(AU32+AV32))</f>
@@ -37326,7 +37326,7 @@
         <v>154</v>
       </c>
       <c r="CR32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CS32" s="156" t="s">
         <v>108</v>
@@ -37339,7 +37339,7 @@
         <v>154</v>
       </c>
       <c r="CY32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CZ32" s="156" t="s">
         <v>108</v>
@@ -38552,10 +38552,10 @@
         <v>204</v>
       </c>
       <c r="BR39" s="154" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
       <c r="BS39" s="153" t="s">
-        <v>10</v>
+        <v>206</v>
       </c>
       <c r="BT39" s="146">
         <f>IF(BR39&lt;5,3,IF(((BQ39-BS39)/BQ39)&lt;-100%,1,IF(((BQ39-BS39)/BQ39)&lt;-50%,2,IF(((BQ39-BS39)/BQ39)&lt;50%,3,IF(((BQ39-BS39)/BQ39)&lt;100%,4,5)))))</f>
@@ -38580,7 +38580,7 @@
         <v/>
       </c>
       <c r="CE39" s="153" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="CF39" s="154" t="s">
         <v>10</v>
@@ -38611,13 +38611,13 @@
         <v/>
       </c>
       <c r="CS39" s="153" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="CT39" s="154" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="CU39" s="153" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="CV39" s="146">
         <f>IF(CT39&lt;5,3,IF(((CS39-CU39)/CS39)&lt;-100%,1,IF(((CS39-CU39)/CS39)&lt;-50%,2,IF(((CS39-CU39)/CS39)&lt;50%,3,IF(((CS39-CU39)/CS39)&lt;100%,4,5)))))</f>
@@ -38642,13 +38642,13 @@
         <v/>
       </c>
       <c r="DG39" s="153" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="DH39" s="154" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="DI39" s="153" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="DJ39" s="146">
         <f>IF(DH39&lt;5,3,IF(((DG39-DI39)/DG39)&lt;-100%,1,IF(((DG39-DI39)/DG39)&lt;-50%,2,IF(((DG39-DI39)/DG39)&lt;50%,3,IF(((DG39-DI39)/DG39)&lt;100%,4,5)))))</f>
@@ -38678,13 +38678,13 @@
         <v/>
       </c>
       <c r="M40" s="155" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N40" s="156" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O40" s="155" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="P40" s="147">
         <f>IF(N40&lt;5,3,IF(((M40-O40)/M40)&lt;-100%,1,IF(((M40-O40)/M40)&lt;-50%,2,IF(((M40-O40)/M40)&lt;50%,3,IF(((M40-O40)/M40)&lt;100%,4,5)))))</f>
@@ -38709,7 +38709,7 @@
         <v/>
       </c>
       <c r="AA40" s="155" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AB40" s="156" t="s">
         <v>10</v>
@@ -38740,13 +38740,13 @@
         <v/>
       </c>
       <c r="AO40" s="155" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AP40" s="156" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AQ40" s="155" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AR40" s="147">
         <f>IF(AP40&lt;5,3,IF(((AO40-AQ40)/AO40)&lt;-100%,1,IF(((AO40-AQ40)/AO40)&lt;-50%,2,IF(((AO40-AQ40)/AO40)&lt;50%,3,IF(((AO40-AQ40)/AO40)&lt;100%,4,5)))))</f>
@@ -38771,7 +38771,7 @@
         <v/>
       </c>
       <c r="BC40" s="155" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="BD40" s="156" t="s">
         <v>10</v>
@@ -38802,13 +38802,13 @@
         <v/>
       </c>
       <c r="BQ40" s="155" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="BR40" s="156" t="s">
-        <v>221</v>
+        <v>10</v>
       </c>
       <c r="BS40" s="155" t="s">
-        <v>222</v>
+        <v>10</v>
       </c>
       <c r="BT40" s="147">
         <f>IF(BR40&lt;5,3,IF(((BQ40-BS40)/BQ40)&lt;-100%,1,IF(((BQ40-BS40)/BQ40)&lt;-50%,2,IF(((BQ40-BS40)/BQ40)&lt;50%,3,IF(((BQ40-BS40)/BQ40)&lt;100%,4,5)))))</f>
@@ -44649,13 +44649,13 @@
         <v>8</v>
       </c>
       <c r="M10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N10" s="154" t="s">
         <v>8</v>
       </c>
       <c r="O10" s="38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P10" s="165" t="n"/>
       <c r="Q10" s="7" t="s">
@@ -44665,13 +44665,13 @@
         <v>8</v>
       </c>
       <c r="S10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T10" s="154" t="s">
         <v>8</v>
       </c>
       <c r="U10" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V10" s="14" t="n"/>
       <c r="W10" s="165" t="n"/>
@@ -44680,7 +44680,7 @@
         <v>96</v>
       </c>
       <c r="Z10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AA10" s="154" t="s">
         <v>8</v>
@@ -44689,14 +44689,14 @@
         <v>9</v>
       </c>
       <c r="AC10" s="38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AD10" s="165" t="n"/>
       <c r="AE10" s="7" t="s">
         <v>96</v>
       </c>
       <c r="AF10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AG10" s="154" t="s">
         <v>8</v>
@@ -44705,7 +44705,7 @@
         <v>9</v>
       </c>
       <c r="AI10" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AJ10" s="14" t="n"/>
       <c r="AL10" s="13" t="n"/>
@@ -44713,13 +44713,13 @@
         <v>96</v>
       </c>
       <c r="AN10" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO10" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="AO10" s="154" t="s">
+      <c r="AP10" s="154" t="s">
         <v>9</v>
-      </c>
-      <c r="AP10" s="154" t="s">
-        <v>8</v>
       </c>
       <c r="AQ10" s="38" t="s">
         <v>8</v>
@@ -44729,13 +44729,13 @@
         <v>96</v>
       </c>
       <c r="AT10" s="154" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU10" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="AU10" s="154" t="s">
+      <c r="AV10" s="154" t="s">
         <v>8</v>
-      </c>
-      <c r="AV10" s="154" t="s">
-        <v>9</v>
       </c>
       <c r="AW10" s="38" t="s">
         <v>8</v>
@@ -44749,13 +44749,13 @@
         <v>9</v>
       </c>
       <c r="BC10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BE10" s="38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BF10" s="165" t="n"/>
       <c r="BG10" s="7" t="s">
@@ -44765,13 +44765,13 @@
         <v>9</v>
       </c>
       <c r="BI10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BJ10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BK10" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BL10" s="14" t="n"/>
       <c r="BN10" s="13" t="n"/>
@@ -44779,7 +44779,7 @@
         <v>96</v>
       </c>
       <c r="BP10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BQ10" s="154" t="s">
         <v>9</v>
@@ -44795,7 +44795,7 @@
         <v>96</v>
       </c>
       <c r="BV10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BW10" s="154" t="s">
         <v>9</v>
@@ -44813,10 +44813,10 @@
         <v>96</v>
       </c>
       <c r="CD10" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE10" s="154" t="s">
         <v>8</v>
-      </c>
-      <c r="CE10" s="154" t="s">
-        <v>9</v>
       </c>
       <c r="CF10" s="154" t="s">
         <v>8</v>
@@ -44829,10 +44829,10 @@
         <v>96</v>
       </c>
       <c r="CJ10" s="154" t="s">
+        <v>8</v>
+      </c>
+      <c r="CK10" s="154" t="s">
         <v>9</v>
-      </c>
-      <c r="CK10" s="154" t="s">
-        <v>8</v>
       </c>
       <c r="CL10" s="154" t="s">
         <v>8</v>
@@ -44846,13 +44846,13 @@
         <v>96</v>
       </c>
       <c r="CR10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="CS10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="CT10" s="154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="CU10" s="38" t="s">
         <v>9</v>
@@ -44862,13 +44862,13 @@
         <v>96</v>
       </c>
       <c r="CX10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="CY10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="CZ10" s="154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="DA10" s="38" t="s">
         <v>9</v>
@@ -44915,32 +44915,32 @@
         <v>97</v>
       </c>
       <c r="L11" s="156" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M11" s="156" t="s">
         <v>103</v>
       </c>
       <c r="N11" s="156" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O11" s="144" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P11" s="75" t="n"/>
       <c r="Q11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="R11" s="156" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S11" s="156" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T11" s="156" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="U11" s="144" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="V11" s="14" t="n"/>
       <c r="W11" s="75" t="n"/>
@@ -44949,32 +44949,32 @@
         <v>97</v>
       </c>
       <c r="Z11" s="156" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AA11" s="156" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AB11" s="156" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AC11" s="144" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="AD11" s="75" t="n"/>
       <c r="AE11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="AF11" s="156" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AG11" s="156" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AH11" s="156" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI11" s="144" t="s">
         <v>102</v>
-      </c>
-      <c r="AI11" s="144" t="s">
-        <v>106</v>
       </c>
       <c r="AJ11" s="14" t="n"/>
       <c r="AL11" s="13" t="n"/>
@@ -44982,32 +44982,32 @@
         <v>97</v>
       </c>
       <c r="AN11" s="156" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AO11" s="156" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AP11" s="156" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AQ11" s="144" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AR11" s="75" t="n"/>
       <c r="AS11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="AT11" s="156" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AU11" s="156" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AV11" s="156" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="AW11" s="144" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AX11" s="14" t="n"/>
       <c r="AZ11" s="13" t="n"/>
@@ -45015,32 +45015,32 @@
         <v>97</v>
       </c>
       <c r="BB11" s="156" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="BC11" s="156" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="BD11" s="156" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="BE11" s="144" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="BF11" s="75" t="n"/>
       <c r="BG11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="BH11" s="156" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="BI11" s="156" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="BJ11" s="156" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="BK11" s="144" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="BL11" s="14" t="n"/>
       <c r="BN11" s="13" t="n"/>
@@ -45048,32 +45048,32 @@
         <v>97</v>
       </c>
       <c r="BP11" s="156" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="BQ11" s="156" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="BR11" s="156" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="BS11" s="144" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="BT11" s="75" t="n"/>
       <c r="BU11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="BV11" s="156" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="BW11" s="156" t="s">
+        <v>100</v>
+      </c>
+      <c r="BX11" s="156" t="s">
         <v>103</v>
       </c>
-      <c r="BX11" s="156" t="s">
-        <v>104</v>
-      </c>
       <c r="BY11" s="144" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BZ11" s="14" t="n"/>
       <c r="CA11" s="75" t="n"/>
@@ -45082,32 +45082,32 @@
         <v>97</v>
       </c>
       <c r="CD11" s="156" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="CE11" s="156" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="CF11" s="156" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="CG11" s="144" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="CH11" s="75" t="n"/>
       <c r="CI11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="CJ11" s="156" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="CK11" s="156" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="CL11" s="156" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="CM11" s="144" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="CN11" s="14" t="n"/>
       <c r="CP11" s="13" t="n"/>
@@ -45115,32 +45115,32 @@
         <v>97</v>
       </c>
       <c r="CR11" s="156" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="CS11" s="156" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="CT11" s="156" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="CU11" s="144" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="CV11" s="75" t="n"/>
       <c r="CW11" s="143" t="s">
         <v>97</v>
       </c>
       <c r="CX11" s="156" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="CY11" s="156" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="CZ11" s="156" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="DA11" s="144" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="DB11" s="14" t="n"/>
       <c r="DD11" s="13" t="n"/>
@@ -48768,7 +48768,7 @@
         <v>109</v>
       </c>
       <c r="AA31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AB31" s="172">
         <f>IF((Z31+AA31)&lt;4,IF(AD4="POS",0.7,IF(AD4="NEUT",0.5,IF(AD4="NEG",0.3,""))),Z31/(Z31+AA31))</f>
@@ -48781,7 +48781,7 @@
         <v>109</v>
       </c>
       <c r="AH31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AI31" s="172">
         <f>IF((AG31+AH31)&lt;4,IF(AD5="POS",0.7,IF(AD5="NEUT",0.5,IF(AD5="NEG",0.3,""))),AG31/(AG31+AH31))</f>
@@ -48793,7 +48793,7 @@
         <v>137</v>
       </c>
       <c r="AN31" s="154" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AO31" s="154" t="s">
         <v>109</v>
@@ -48806,7 +48806,7 @@
         <v>137</v>
       </c>
       <c r="AU31" s="154" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AV31" s="154" t="s">
         <v>109</v>
@@ -48905,10 +48905,10 @@
         <v>137</v>
       </c>
       <c r="CR31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="CS31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="CT31" s="172">
         <f>IF((CR31+CS31)&lt;4,IF(CV4="POS",0.7,IF(CV4="NEUT",0.5,IF(CV4="NEG",0.3,""))),CR31/(CR31+CS31))</f>
@@ -48918,10 +48918,10 @@
         <v>137</v>
       </c>
       <c r="CY31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="CZ31" s="154" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="DA31" s="172">
         <f>IF((CY31+CZ31)&lt;4,IF(CV5="POS",0.7,IF(CV5="NEUT",0.5,IF(CV5="NEG",0.3,""))),CY31/(CY31+CZ31))</f>
@@ -48980,10 +48980,10 @@
         <v>154</v>
       </c>
       <c r="L32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M32" s="156" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="N32" s="170">
         <f>IF((L32+M32)&lt;4,IF(P4="POS",0.7,IF(P4="NEUT",0.5,IF(P4="NEG",0.3,""))),L32/(L32+M32))</f>
@@ -48993,10 +48993,10 @@
         <v>154</v>
       </c>
       <c r="S32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="T32" s="156" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="U32" s="170">
         <f>IF((S32+T32)&lt;4,IF(P5="POS",0.7,IF(P5="NEUT",0.5,IF(P5="NEG",0.3,""))),S32/(S32+T32))</f>
@@ -49039,7 +49039,7 @@
         <v>98</v>
       </c>
       <c r="AO32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AP32" s="170">
         <f>IF((AN32+AO32)&lt;4,IF(AR4="POS",0.7,IF(AR4="NEUT",0.5,IF(AR4="NEG",0.3,""))),AN32/(AN32+AO32))</f>
@@ -49052,7 +49052,7 @@
         <v>98</v>
       </c>
       <c r="AV32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AW32" s="170">
         <f>IF((AU32+AV32)&lt;4,IF(AR5="POS",0.7,IF(AR5="NEUT",0.5,IF(AR5="NEG",0.3,""))),AU32/(AU32+AV32))</f>
@@ -49064,10 +49064,10 @@
         <v>154</v>
       </c>
       <c r="BB32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="BC32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="BD32" s="170">
         <f>IF((BB32+BC32)&lt;4,IF(BF4="POS",0.7,IF(BF4="NEUT",0.5,IF(BF4="NEG",0.3,""))),BB32/(BB32+BC32))</f>
@@ -49077,10 +49077,10 @@
         <v>154</v>
       </c>
       <c r="BI32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="BJ32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="BK32" s="170">
         <f>IF((BI32+BJ32)&lt;4,IF(BF5="POS",0.7,IF(BF5="NEUT",0.5,IF(BF5="NEG",0.3,""))),BI32/(BI32+BJ32))</f>
@@ -49095,7 +49095,7 @@
         <v>108</v>
       </c>
       <c r="BQ32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="BR32" s="170">
         <f>IF((BP32+BQ32)&lt;4,IF(BT4="POS",0.7,IF(BT4="NEUT",0.5,IF(BT4="NEG",0.3,""))),BP32/(BP32+BQ32))</f>
@@ -49108,7 +49108,7 @@
         <v>108</v>
       </c>
       <c r="BX32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="BY32" s="170">
         <f>IF((BW32+BX32)&lt;4,IF(BT5="POS",0.7,IF(BT5="NEUT",0.5,IF(BT5="NEG",0.3,""))),BW32/(BW32+BX32))</f>
@@ -49120,7 +49120,7 @@
         <v>154</v>
       </c>
       <c r="CD32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CE32" s="156" t="s">
         <v>185</v>
@@ -49133,7 +49133,7 @@
         <v>154</v>
       </c>
       <c r="CK32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CL32" s="156" t="s">
         <v>185</v>
@@ -49148,10 +49148,10 @@
         <v>154</v>
       </c>
       <c r="CR32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CS32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CT32" s="170">
         <f>IF((CR32+CS32)&lt;4,IF(CV4="POS",0.7,IF(CV4="NEUT",0.5,IF(CV4="NEG",0.3,""))),CR32/(CR32+CS32))</f>
@@ -49161,10 +49161,10 @@
         <v>154</v>
       </c>
       <c r="CY32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="CZ32" s="156" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="DA32" s="170">
         <f>IF((CY32+CZ32)&lt;4,IF(CV5="POS",0.7,IF(CV5="NEUT",0.5,IF(CV5="NEG",0.3,""))),CY32/(CY32+CZ32))</f>
@@ -50317,10 +50317,10 @@
         <v>304</v>
       </c>
       <c r="BD39" s="154" t="s">
+        <v>197</v>
+      </c>
+      <c r="BE39" s="153" t="s">
         <v>305</v>
-      </c>
-      <c r="BE39" s="153" t="s">
-        <v>306</v>
       </c>
       <c r="BF39" s="146">
         <f>IF(BD39&lt;5,3,IF(((BC39-BE39)/BC39)&lt;-100%,1,IF(((BC39-BE39)/BC39)&lt;-50%,2,IF(((BC39-BE39)/BC39)&lt;50%,3,IF(((BC39-BE39)/BC39)&lt;100%,4,5)))))</f>
@@ -50345,13 +50345,13 @@
         <v/>
       </c>
       <c r="BQ39" s="153" t="s">
+        <v>306</v>
+      </c>
+      <c r="BR39" s="154" t="s">
         <v>307</v>
       </c>
-      <c r="BR39" s="154" t="s">
-        <v>10</v>
-      </c>
       <c r="BS39" s="153" t="s">
-        <v>10</v>
+        <v>223</v>
       </c>
       <c r="BT39" s="146">
         <f>IF(BR39&lt;5,3,IF(((BQ39-BS39)/BQ39)&lt;-100%,1,IF(((BQ39-BS39)/BQ39)&lt;-50%,2,IF(((BQ39-BS39)/BQ39)&lt;50%,3,IF(((BQ39-BS39)/BQ39)&lt;100%,4,5)))))</f>
@@ -50410,10 +50410,10 @@
         <v>309</v>
       </c>
       <c r="CT39" s="154" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
       <c r="CU39" s="153" t="s">
-        <v>310</v>
+        <v>10</v>
       </c>
       <c r="CV39" s="146">
         <f>IF(CT39&lt;5,3,IF(((CS39-CU39)/CS39)&lt;-100%,1,IF(((CS39-CU39)/CS39)&lt;-50%,2,IF(((CS39-CU39)/CS39)&lt;50%,3,IF(((CS39-CU39)/CS39)&lt;100%,4,5)))))</f>
@@ -50465,7 +50465,7 @@
         <v/>
       </c>
       <c r="M40" s="155" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N40" s="156" t="s">
         <v>10</v>
@@ -50496,7 +50496,7 @@
         <v/>
       </c>
       <c r="AA40" s="155" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB40" s="156" t="s">
         <v>10</v>
@@ -50527,7 +50527,7 @@
         <v/>
       </c>
       <c r="AO40" s="155" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AP40" s="156" t="s">
         <v>10</v>
@@ -50558,10 +50558,10 @@
         <v/>
       </c>
       <c r="BC40" s="155" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD40" s="156" t="s">
         <v>314</v>
-      </c>
-      <c r="BD40" s="156" t="s">
-        <v>213</v>
       </c>
       <c r="BE40" s="155" t="s">
         <v>315</v>
@@ -50592,10 +50592,10 @@
         <v>316</v>
       </c>
       <c r="BR40" s="156" t="s">
-        <v>317</v>
+        <v>10</v>
       </c>
       <c r="BS40" s="155" t="s">
-        <v>205</v>
+        <v>10</v>
       </c>
       <c r="BT40" s="147">
         <f>IF(BR40&lt;5,3,IF(((BQ40-BS40)/BQ40)&lt;-100%,1,IF(((BQ40-BS40)/BQ40)&lt;-50%,2,IF(((BQ40-BS40)/BQ40)&lt;50%,3,IF(((BQ40-BS40)/BQ40)&lt;100%,4,5)))))</f>
@@ -50620,7 +50620,7 @@
         <v/>
       </c>
       <c r="CE40" s="155" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CF40" s="156" t="s">
         <v>10</v>
@@ -50651,13 +50651,13 @@
         <v/>
       </c>
       <c r="CS40" s="155" t="s">
+        <v>318</v>
+      </c>
+      <c r="CT40" s="156" t="s">
+        <v>212</v>
+      </c>
+      <c r="CU40" s="155" t="s">
         <v>319</v>
-      </c>
-      <c r="CT40" s="156" t="s">
-        <v>10</v>
-      </c>
-      <c r="CU40" s="155" t="s">
-        <v>10</v>
       </c>
       <c r="CV40" s="147">
         <f>IF(CT40&lt;5,3,IF(((CS40-CU40)/CS40)&lt;-100%,1,IF(((CS40-CU40)/CS40)&lt;-50%,2,IF(((CS40-CU40)/CS40)&lt;50%,3,IF(((CS40-CU40)/CS40)&lt;100%,4,5)))))</f>

</xml_diff>